<commit_message>
Add page metadata header and expand language section button to cover the whole language section heading
</commit_message>
<xml_diff>
--- a/data/page_metadata.xlsx
+++ b/data/page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\Portfolio Website\portfolio-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CE5A59-E3AF-4A55-9BF8-477601B254A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293DDBEF-994A-4055-B6E4-D369887BA8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="121">
   <si>
     <t>home</t>
   </si>
@@ -129,24 +129,12 @@
     <t>pandas, matplotlib, sqlite, sqlalchemy, flask</t>
   </si>
   <si>
-    <t>python, html, css</t>
-  </si>
-  <si>
     <t>database</t>
   </si>
   <si>
-    <t>javascript, html, css</t>
-  </si>
-  <si>
     <t>bootstrap</t>
   </si>
   <si>
-    <t>UFO Sightings Website</t>
-  </si>
-  <si>
-    <t>Belly Button Biodiversity Dashboard</t>
-  </si>
-  <si>
     <t>bootstrap, d3, plotly</t>
   </si>
   <si>
@@ -183,18 +171,9 @@
     <t>pandas, sklearn, imblearn</t>
   </si>
   <si>
-    <t>resampling: oversampling, undersampling, combination sampling ensemble methods: random forest, AdaBoost</t>
-  </si>
-  <si>
     <t>pandas, sklearn</t>
   </si>
   <si>
-    <t>PCA, K-Means Clustering</t>
-  </si>
-  <si>
-    <t>python, javascript, html, css</t>
-  </si>
-  <si>
     <t>app</t>
   </si>
   <si>
@@ -204,18 +183,12 @@
     <t>database, web scraping, app, logistic regression, PCA</t>
   </si>
   <si>
-    <t>python, css</t>
-  </si>
-  <si>
     <t>pandas, httpx, selectolax</t>
   </si>
   <si>
     <t>pandas, splinter, selectolax, spacy</t>
   </si>
   <si>
-    <t>webs craping, OOP, NLP</t>
-  </si>
-  <si>
     <t>web scraping</t>
   </si>
   <si>
@@ -288,9 +261,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>main_tools</t>
-  </si>
-  <si>
     <t>website</t>
   </si>
   <si>
@@ -375,13 +345,49 @@
     <t>sidebar</t>
   </si>
   <si>
-    <t>repo_link</t>
-  </si>
-  <si>
-    <t>languages_used</t>
-  </si>
-  <si>
     <t>concepts</t>
+  </si>
+  <si>
+    <t>languages</t>
+  </si>
+  <si>
+    <t>repo</t>
+  </si>
+  <si>
+    <t>webs scraping, OOP, NLP</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Python, CSS</t>
+  </si>
+  <si>
+    <t>Python, HTML, CSS</t>
+  </si>
+  <si>
+    <t>JavaScript, HTML, CSS</t>
+  </si>
+  <si>
+    <t>Markdown</t>
+  </si>
+  <si>
+    <t>Python, JavaScript, HTML, CSS</t>
+  </si>
+  <si>
+    <t>PCA, k-means clustering</t>
+  </si>
+  <si>
+    <t>https://cdpeters.github.io/biodiversity-dashboard-plotly/</t>
+  </si>
+  <si>
+    <t>https://cdpeters.github.io/dynamic-UFO-website-javascript/</t>
+  </si>
+  <si>
+    <t>libraries_tools</t>
+  </si>
+  <si>
+    <t>resampling, ensemble methods</t>
   </si>
 </sst>
 </file>
@@ -784,7 +790,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -795,7 +801,7 @@
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="61.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="86" style="1" customWidth="1"/>
     <col min="9" max="9" width="66" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.88671875" style="1" bestFit="1" customWidth="1"/>
@@ -804,34 +810,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -883,19 +889,19 @@
         <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -912,24 +918,24 @@
         <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B6" s="1" t="b">
         <v>1</v>
@@ -941,24 +947,24 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="34.799999999999997" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B7" s="1" t="b">
         <v>1</v>
@@ -970,24 +976,24 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B8" s="1" t="b">
         <v>1</v>
@@ -999,24 +1005,24 @@
         <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B9" s="1" t="b">
         <v>1</v>
@@ -1031,21 +1037,21 @@
         <v>13</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="b">
         <v>1</v>
@@ -1060,10 +1066,10 @@
         <v>16</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>29</v>
@@ -1074,7 +1080,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="b">
         <v>1</v>
@@ -1089,10 +1095,10 @@
         <v>17</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>28</v>
@@ -1103,7 +1109,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B12" s="1" t="b">
         <v>1</v>
@@ -1118,10 +1124,10 @@
         <v>14</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>26</v>
@@ -1129,7 +1135,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B13" s="1" t="b">
         <v>1</v>
@@ -1144,10 +1150,10 @@
         <v>18</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1168,7 +1174,7 @@
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="1" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>25</v>
@@ -1176,7 +1182,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B15" s="1" t="b">
         <v>1</v>
@@ -1185,22 +1191,22 @@
         <v>13</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -1214,27 +1220,27 @@
         <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="b">
         <v>1</v>
@@ -1243,27 +1249,27 @@
         <v>15</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B18" s="1" t="b">
         <v>1</v>
@@ -1272,27 +1278,27 @@
         <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B19" s="1" t="b">
         <v>1</v>
@@ -1301,13 +1307,13 @@
         <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>31</v>
@@ -1316,12 +1322,12 @@
         <v>32</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B20" s="1" t="b">
         <v>1</v>
@@ -1330,30 +1336,30 @@
         <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B21" s="1" t="b">
         <v>1</v>
@@ -1362,27 +1368,27 @@
         <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="J21" s="3" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B22" s="1" t="b">
         <v>1</v>
@@ -1391,25 +1397,25 @@
         <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>38</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -1429,7 +1435,7 @@
         <v>21</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>24</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add some missing data to page_metadata excel file and use longest string for libraries_tools to test app sizing
</commit_message>
<xml_diff>
--- a/data/page_metadata.xlsx
+++ b/data/page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\Portfolio Website\portfolio-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293DDBEF-994A-4055-B6E4-D369887BA8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1D983C-B2F2-4A63-821F-881E0DEFFA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="124">
   <si>
     <t>home</t>
   </si>
@@ -267,9 +267,6 @@
     <t>javascript</t>
   </si>
   <si>
-    <t>https://github.com/cdpeters/portfolio-website</t>
-  </si>
-  <si>
     <t>https://github.com/cdpeters/handbell-music-validation</t>
   </si>
   <si>
@@ -388,6 +385,18 @@
   </si>
   <si>
     <t>resampling, ensemble methods</t>
+  </si>
+  <si>
+    <t>pandas</t>
+  </si>
+  <si>
+    <t>https://github.com/cdpeters/portfolio-website/blob/main/tools.py</t>
+  </si>
+  <si>
+    <t>https://github.com/cdpeters/dash-test-app</t>
+  </si>
+  <si>
+    <t>https://github.com/cdpeters/portfolio-website/tree/main/notes</t>
   </si>
 </sst>
 </file>
@@ -445,7 +454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -467,6 +476,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -813,7 +823,7 @@
         <v>76</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>75</v>
@@ -825,16 +835,16 @@
         <v>77</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>78</v>
@@ -889,13 +899,13 @@
         <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>52</v>
@@ -918,19 +928,19 @@
         <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>53</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -947,19 +957,19 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>48</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -976,19 +986,19 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>47</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1005,13 +1015,13 @@
         <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>40</v>
@@ -1037,10 +1047,10 @@
         <v>13</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>33</v>
@@ -1066,10 +1076,10 @@
         <v>16</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>29</v>
@@ -1095,10 +1105,10 @@
         <v>17</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>28</v>
@@ -1124,10 +1134,10 @@
         <v>14</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>26</v>
@@ -1150,10 +1160,13 @@
         <v>18</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1172,9 +1185,11 @@
       <c r="E14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="11" t="s">
+        <v>121</v>
+      </c>
       <c r="G14" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>25</v>
@@ -1182,7 +1197,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" s="1" t="b">
         <v>1</v>
@@ -1194,13 +1209,13 @@
         <v>78</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>56</v>
@@ -1226,10 +1241,10 @@
         <v>7</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>50</v>
@@ -1255,7 +1270,7 @@
         <v>8</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>44</v>
@@ -1284,10 +1299,10 @@
         <v>9</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>42</v>
@@ -1313,7 +1328,7 @@
         <v>15</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>31</v>
@@ -1342,10 +1357,10 @@
         <v>10</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>38</v>
@@ -1374,16 +1389,16 @@
         <v>11</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -1403,10 +1418,10 @@
         <v>12</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>35</v>
@@ -1415,7 +1430,7 @@
         <v>49</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -1434,8 +1449,11 @@
       <c r="E23" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="F23" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="G23" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1460,8 +1478,10 @@
     <hyperlink ref="F16" r:id="rId18" xr:uid="{E267236B-DF79-4652-AA09-481309B98BE1}"/>
     <hyperlink ref="J22" r:id="rId19" xr:uid="{E6B871A8-109A-4EE5-9BD7-70659F069CB1}"/>
     <hyperlink ref="J21" r:id="rId20" xr:uid="{FB928050-0DA6-4298-AC87-1B73E4384C08}"/>
+    <hyperlink ref="F14" r:id="rId21" xr:uid="{FF316A68-48F2-4723-94D4-BDFC6FC1C12F}"/>
+    <hyperlink ref="F23" r:id="rId22" xr:uid="{AB90E9EA-AEFF-4EF8-A322-CAF589A0B570}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId21"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add sidebar to the data_types so that its type is explicit
</commit_message>
<xml_diff>
--- a/data/page_metadata.xlsx
+++ b/data/page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\Portfolio Website\portfolio-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1D983C-B2F2-4A63-821F-881E0DEFFA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438AAD4B-99B0-4EB6-867D-CA354346AC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -800,21 +800,21 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="86" style="1" customWidth="1"/>
-    <col min="9" max="9" width="66" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="90" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="58.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="52.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Remove all filler pages
</commit_message>
<xml_diff>
--- a/data/page_metadata.xlsx
+++ b/data/page_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\Portfolio Website\portfolio-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438AAD4B-99B0-4EB6-867D-CA354346AC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70F043E-CDE1-4EC1-A997-66F7D48FF486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="125">
   <si>
     <t>home</t>
   </si>
@@ -102,9 +102,6 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>click</t>
-  </si>
-  <si>
     <t>pandas, matplotlib</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>bootstrap, d3, plotly</t>
   </si>
   <si>
-    <t>index.html file</t>
-  </si>
-  <si>
     <t>leaflet, d3, mapbox</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>pandas, tableau</t>
   </si>
   <si>
-    <t>tableau public visualization</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -195,9 +186,6 @@
     <t>database, app</t>
   </si>
   <si>
-    <t>pandas, dash, ibis, sqlite, tailwindcss</t>
-  </si>
-  <si>
     <t>crypto_unsupervised</t>
   </si>
   <si>
@@ -397,6 +385,21 @@
   </si>
   <si>
     <t>https://github.com/cdpeters/portfolio-website/tree/main/notes</t>
+  </si>
+  <si>
+    <t>https://public.tableau.com/views/NYC_CitiBike_Challenge_16506220556720/August2019NYCCitibikeStudy?:language=en-US&amp;:display_count=n&amp;:origin=viz_share_link</t>
+  </si>
+  <si>
+    <t>click, subprocess</t>
+  </si>
+  <si>
+    <t>CLI</t>
+  </si>
+  <si>
+    <t>cli</t>
+  </si>
+  <si>
+    <t>pandas, dash, ibis-framework, sqlite, tailwindcss</t>
   </si>
 </sst>
 </file>
@@ -799,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2C412C-6E97-4788-869B-F51667F527C3}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -820,34 +823,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -876,9 +879,6 @@
       <c r="C3" s="10">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
@@ -899,19 +899,19 @@
         <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -928,24 +928,24 @@
         <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B6" s="1" t="b">
         <v>1</v>
@@ -957,24 +957,24 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1" t="b">
         <v>1</v>
@@ -986,24 +986,24 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1" t="b">
         <v>1</v>
@@ -1015,24 +1015,24 @@
         <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="b">
         <v>1</v>
@@ -1047,21 +1047,21 @@
         <v>13</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B10" s="1" t="b">
         <v>1</v>
@@ -1076,21 +1076,21 @@
         <v>16</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B11" s="1" t="b">
         <v>1</v>
@@ -1105,21 +1105,21 @@
         <v>17</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B12" s="1" t="b">
         <v>1</v>
@@ -1134,18 +1134,18 @@
         <v>14</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B13" s="1" t="b">
         <v>1</v>
@@ -1160,13 +1160,13 @@
         <v>18</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1180,24 +1180,27 @@
         <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>25</v>
+      <c r="I14" s="4" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B15" s="1" t="b">
         <v>1</v>
@@ -1206,22 +1209,22 @@
         <v>13</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>56</v>
+        <v>124</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -1235,27 +1238,27 @@
         <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B17" s="1" t="b">
         <v>1</v>
@@ -1264,27 +1267,27 @@
         <v>15</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B18" s="1" t="b">
         <v>1</v>
@@ -1293,27 +1296,27 @@
         <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B19" s="1" t="b">
         <v>1</v>
@@ -1322,27 +1325,27 @@
         <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="I19" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B20" s="1" t="b">
         <v>1</v>
@@ -1351,30 +1354,27 @@
         <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J20" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B21" s="1" t="b">
         <v>1</v>
@@ -1383,27 +1383,27 @@
         <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B22" s="1" t="b">
         <v>1</v>
@@ -1412,25 +1412,25 @@
         <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -1450,10 +1450,10 @@
         <v>21</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1480,8 +1480,9 @@
     <hyperlink ref="J21" r:id="rId20" xr:uid="{FB928050-0DA6-4298-AC87-1B73E4384C08}"/>
     <hyperlink ref="F14" r:id="rId21" xr:uid="{FF316A68-48F2-4723-94D4-BDFC6FC1C12F}"/>
     <hyperlink ref="F23" r:id="rId22" xr:uid="{AB90E9EA-AEFF-4EF8-A322-CAF589A0B570}"/>
+    <hyperlink ref="J18" r:id="rId23" xr:uid="{1131C430-A06F-4FC5-A6FA-F09DFC8A795F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId23"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add the dash test app and nba prediction final project pages
</commit_message>
<xml_diff>
--- a/data/page_metadata.xlsx
+++ b/data/page_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\Portfolio Website\portfolio-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C447F283-6B7E-4EFE-81B4-2AD2E5E26B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526A7F56-F3C7-4461-AAEF-0EB28F3BFDE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
   <si>
     <t>home</t>
   </si>
@@ -181,6 +181,42 @@
   </si>
   <si>
     <t>school_district</t>
+  </si>
+  <si>
+    <t>dash_test_app</t>
+  </si>
+  <si>
+    <t>Dash Test App</t>
+  </si>
+  <si>
+    <t>https://github.com/cdpeters/dash-test-app</t>
+  </si>
+  <si>
+    <t>Python, CSS</t>
+  </si>
+  <si>
+    <t>pandas, dash, ibis-framework, sqlite, tailwindcss</t>
+  </si>
+  <si>
+    <t>database, app</t>
+  </si>
+  <si>
+    <t>nba_prediction</t>
+  </si>
+  <si>
+    <t>NBA Prediction</t>
+  </si>
+  <si>
+    <t>https://github.com/pascalegeday/NBA_Prediction_Analysis</t>
+  </si>
+  <si>
+    <t>Python, JavaScript, HTML, CSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pandas, splinter, bs4 (beautiful soup 4), sqlalchemy, bootstrap, AWS, postgresql, flask </t>
+  </si>
+  <si>
+    <t>database, web scraping, app, logistic regression, PCA</t>
   </si>
 </sst>
 </file>
@@ -238,7 +274,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -251,6 +287,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -571,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2C412C-6E97-4788-869B-F51667F527C3}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -835,6 +880,58 @@
         <v>48</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="7">
+        <v>9</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="7">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{9D280C85-D79B-4336-9A15-038EBEDAD179}"/>
@@ -845,8 +942,10 @@
     <hyperlink ref="E8" r:id="rId6" xr:uid="{0BBE72C1-DD83-47AD-9C3F-1663B75D12A2}"/>
     <hyperlink ref="E9" r:id="rId7" xr:uid="{5DEC456C-D3DE-4127-A58F-AB908A1F6435}"/>
     <hyperlink ref="E10" r:id="rId8" xr:uid="{08DF44EB-DC79-4D92-A240-4E05E17FBDF7}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{DFA5D084-673E-4D85-BBCF-AEC96AB4B5D1}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{3594118F-A025-4375-8B1A-478101EBBD1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correct image src attributes and clean up nba prediction report
</commit_message>
<xml_diff>
--- a/data/page_metadata.xlsx
+++ b/data/page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\Portfolio Website\portfolio-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526A7F56-F3C7-4461-AAEF-0EB28F3BFDE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F6F514-24B2-4680-BEE5-D0A6748B1103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
+    <workbookView xWindow="3132" yWindow="2628" windowWidth="17280" windowHeight="9072" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
   <si>
-    <t>home</t>
-  </si>
-  <si>
-    <t>Home</t>
-  </si>
-  <si>
     <t>python</t>
   </si>
   <si>
@@ -217,6 +211,12 @@
   </si>
   <si>
     <t>database, web scraping, app, logistic regression, PCA</t>
+  </si>
+  <si>
+    <t>about_me</t>
+  </si>
+  <si>
+    <t>About Me</t>
   </si>
 </sst>
 </file>
@@ -619,7 +619,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -638,298 +638,298 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="B2" s="7">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="7">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="7">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="H4" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="7">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="7">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="7">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="7">
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="H8" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B9" s="7">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B10" s="7">
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B11" s="7">
         <v>9</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="G11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="H11" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B12" s="7">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="G12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify the project summary website row to show a link if there is a website
</commit_message>
<xml_diff>
--- a/data/page_metadata.xlsx
+++ b/data/page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\Portfolio Website\portfolio-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F6F514-24B2-4680-BEE5-D0A6748B1103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DED8DE-13C8-4D55-8C82-BE3D39080D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3132" yWindow="2628" windowWidth="17280" windowHeight="9072" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="85">
   <si>
     <t>python</t>
   </si>
@@ -217,6 +217,69 @@
   </si>
   <si>
     <t>About Me</t>
+  </si>
+  <si>
+    <t>linear regression, t-test, hypothesis testing, study design</t>
+  </si>
+  <si>
+    <t>dplyr</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>https://github.com/cdpeters/MechaCar-statistical-analysis-R</t>
+  </si>
+  <si>
+    <t>MechaCar Statistics</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>mechacar</t>
+  </si>
+  <si>
+    <t>https://public.tableau.com/views/NYC_CitiBike_Challenge_16506220556720/August2019NYCCitibikeStudy?:language=en-US&amp;:display_count=n&amp;:origin=viz_share_link</t>
+  </si>
+  <si>
+    <t>pandas, tableau</t>
+  </si>
+  <si>
+    <t>https://github.com/cdpeters/bike-sharing-tableau</t>
+  </si>
+  <si>
+    <t>Bike Sharing</t>
+  </si>
+  <si>
+    <t>tableau</t>
+  </si>
+  <si>
+    <t>bike_sharing</t>
+  </si>
+  <si>
+    <t>website_name</t>
+  </si>
+  <si>
+    <t>NYC CitiBike Challenge</t>
+  </si>
+  <si>
+    <t>postgresql</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>https://github.com/cdpeters/employee-database-postgresql</t>
+  </si>
+  <si>
+    <t>Employee Database</t>
+  </si>
+  <si>
+    <t>sql</t>
+  </si>
+  <si>
+    <t>employee_db</t>
   </si>
 </sst>
 </file>
@@ -616,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2C412C-6E97-4788-869B-F51667F527C3}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -633,10 +696,11 @@
     <col min="7" max="7" width="90" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="58.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="52.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -664,8 +728,11 @@
       <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
@@ -678,7 +745,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -704,7 +771,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -730,7 +797,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -756,7 +823,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -782,7 +849,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -808,7 +875,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -834,7 +901,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
@@ -857,7 +924,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
@@ -880,7 +947,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>50</v>
       </c>
@@ -906,7 +973,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>56</v>
       </c>
@@ -930,6 +997,87 @@
       </c>
       <c r="H12" s="4" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="7">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="7">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="7">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -944,8 +1092,12 @@
     <hyperlink ref="E10" r:id="rId8" xr:uid="{08DF44EB-DC79-4D92-A240-4E05E17FBDF7}"/>
     <hyperlink ref="E11" r:id="rId9" xr:uid="{DFA5D084-673E-4D85-BBCF-AEC96AB4B5D1}"/>
     <hyperlink ref="E12" r:id="rId10" xr:uid="{3594118F-A025-4375-8B1A-478101EBBD1E}"/>
+    <hyperlink ref="E13" r:id="rId11" xr:uid="{C97D4B86-4F17-4BE5-8771-40E4B8A8781F}"/>
+    <hyperlink ref="E14" r:id="rId12" xr:uid="{D4592C7E-1F81-49BA-8CD3-AEC64D82E9B6}"/>
+    <hyperlink ref="I14" r:id="rId13" xr:uid="{9F657C65-7C4B-4A61-9A28-012A2D8E8603}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{31227D6A-73B4-49CC-8654-EDFA7CEF3BA3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modify and generate new page metadata
</commit_message>
<xml_diff>
--- a/data/page_metadata.xlsx
+++ b/data/page_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\Portfolio Website\portfolio-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DED8DE-13C8-4D55-8C82-BE3D39080D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB044C40-1D12-4A81-88C4-06FA5903BB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0F48850E-ADBC-4F08-8282-8BC2E517D1A7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="116">
   <si>
     <t>python</t>
   </si>
@@ -198,21 +198,6 @@
     <t>nba_prediction</t>
   </si>
   <si>
-    <t>NBA Prediction</t>
-  </si>
-  <si>
-    <t>https://github.com/pascalegeday/NBA_Prediction_Analysis</t>
-  </si>
-  <si>
-    <t>Python, JavaScript, HTML, CSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pandas, splinter, bs4 (beautiful soup 4), sqlalchemy, bootstrap, AWS, postgresql, flask </t>
-  </si>
-  <si>
-    <t>database, web scraping, app, logistic regression, PCA</t>
-  </si>
-  <si>
     <t>about_me</t>
   </si>
   <si>
@@ -280,6 +265,114 @@
   </si>
   <si>
     <t>employee_db</t>
+  </si>
+  <si>
+    <t>NBA Champion Analysis</t>
+  </si>
+  <si>
+    <t>https://github.com/cdpeters/nba-prediction-analysis</t>
+  </si>
+  <si>
+    <t>Python, HTML, CSS, Tableau</t>
+  </si>
+  <si>
+    <t>pandas, flask, flask-sqlalchemy, flask-caching, sqlalchemy, selectolax, selenium, beautifulsoup4, seaborn, python-dotenv, scikit-learn, ibis-framework, AWS, railway.app</t>
+  </si>
+  <si>
+    <t>database, web scraping, app, logistic regression, PCA, exploratory analysis</t>
+  </si>
+  <si>
+    <t>https://nba-champion-analysis.up.railway.app/</t>
+  </si>
+  <si>
+    <t>dev_tool_cli</t>
+  </si>
+  <si>
+    <t>cli</t>
+  </si>
+  <si>
+    <t>Dev Tool CLI</t>
+  </si>
+  <si>
+    <t>https://github.com/cdpeters/portfolio-website/blob/main/tools.py</t>
+  </si>
+  <si>
+    <t>click, subprocess</t>
+  </si>
+  <si>
+    <t>CLI</t>
+  </si>
+  <si>
+    <t>map_earthquakes</t>
+  </si>
+  <si>
+    <t>javascript</t>
+  </si>
+  <si>
+    <t>Mapping Earthquakes</t>
+  </si>
+  <si>
+    <t>https://github.com/cdpeters/mapping-earthquakes-leaflet</t>
+  </si>
+  <si>
+    <t>JavaScript, HTML, CSS</t>
+  </si>
+  <si>
+    <t>leaflet, d3, mapbox</t>
+  </si>
+  <si>
+    <t>Mapbox API</t>
+  </si>
+  <si>
+    <t>biodiversity</t>
+  </si>
+  <si>
+    <t>Biodiversity Dashboard</t>
+  </si>
+  <si>
+    <t>https://github.com/cdpeters/biodiversity-dashboard-plotly</t>
+  </si>
+  <si>
+    <t>bootstrap, d3, plotly</t>
+  </si>
+  <si>
+    <t>https://cdpeters.github.io/biodiversity-dashboard-plotly/</t>
+  </si>
+  <si>
+    <t>ufo_sightings</t>
+  </si>
+  <si>
+    <t>UFO Sightings</t>
+  </si>
+  <si>
+    <t>https://github.com/cdpeters/dynamic-UFO-website-javascript</t>
+  </si>
+  <si>
+    <t>bootstrap</t>
+  </si>
+  <si>
+    <t>app</t>
+  </si>
+  <si>
+    <t>https://cdpeters.github.io/dynamic-UFO-website-javascript/</t>
+  </si>
+  <si>
+    <t>guides</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>Setup/Workflow Guides</t>
+  </si>
+  <si>
+    <t>https://github.com/cdpeters/portfolio-website/tree/main/notes</t>
+  </si>
+  <si>
+    <t>Markdown</t>
+  </si>
+  <si>
+    <t>documentation, project setup, workflows</t>
   </si>
 </sst>
 </file>
@@ -337,7 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -359,6 +452,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -679,24 +773,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2C412C-6E97-4788-869B-F51667F527C3}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="63" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="90" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="75" style="4" customWidth="1"/>
     <col min="8" max="8" width="58.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="52.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -719,7 +813,7 @@
       <c r="F1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="6" t="s">
@@ -729,18 +823,18 @@
         <v>7</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B2" s="7">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -764,7 +858,7 @@
       <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="4" t="s">
@@ -790,7 +884,7 @@
       <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="4" t="s">
@@ -816,7 +910,7 @@
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -842,7 +936,7 @@
       <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H6" s="4" t="s">
@@ -868,7 +962,7 @@
       <c r="F7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H7" s="4" t="s">
@@ -894,7 +988,7 @@
       <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H8" s="4" t="s">
@@ -920,7 +1014,7 @@
       <c r="F9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -943,7 +1037,7 @@
       <c r="F10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -966,14 +1060,14 @@
       <c r="F11" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="10" t="s">
         <v>54</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="52.2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>56</v>
       </c>
@@ -984,100 +1078,243 @@
         <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>60</v>
+        <v>82</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>61</v>
+        <v>84</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B13" s="7">
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B14" s="7">
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>72</v>
+      <c r="G14" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B15" s="7">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="7">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="7">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="7">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="7">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="7">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1096,8 +1333,16 @@
     <hyperlink ref="E14" r:id="rId12" xr:uid="{D4592C7E-1F81-49BA-8CD3-AEC64D82E9B6}"/>
     <hyperlink ref="I14" r:id="rId13" xr:uid="{9F657C65-7C4B-4A61-9A28-012A2D8E8603}"/>
     <hyperlink ref="E15" r:id="rId14" xr:uid="{31227D6A-73B4-49CC-8654-EDFA7CEF3BA3}"/>
+    <hyperlink ref="I12" r:id="rId15" xr:uid="{1B953180-0FFE-4C5F-864A-6BAAD97C1C06}"/>
+    <hyperlink ref="E16" r:id="rId16" xr:uid="{1C554EC0-F00A-43F4-8835-9026917B0DAA}"/>
+    <hyperlink ref="E17" r:id="rId17" xr:uid="{5DC278CA-58BA-4869-993E-EFCED176BC66}"/>
+    <hyperlink ref="E18" r:id="rId18" xr:uid="{76992F90-2A53-4B12-B9F8-0FE00BE22385}"/>
+    <hyperlink ref="I18" r:id="rId19" xr:uid="{A0455F4C-62DE-4375-A61D-FCFC45FE70B4}"/>
+    <hyperlink ref="E19" r:id="rId20" xr:uid="{3DA97EF0-4E20-4D79-AA49-98677FFD5404}"/>
+    <hyperlink ref="I19" r:id="rId21" xr:uid="{AFC25449-4BF1-41AC-BA86-A7F8A4614DCE}"/>
+    <hyperlink ref="E20" r:id="rId22" xr:uid="{0B43302E-7669-49DC-BA1D-25CECB4B6EFB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>